<commit_message>
adding mock backend and change some layout
</commit_message>
<xml_diff>
--- a/data-employee.xlsx
+++ b/data-employee.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14925" windowHeight="4575"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14925" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="87">
   <si>
     <t>no</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Johnny</t>
   </si>
   <si>
-    <t>england</t>
-  </si>
-  <si>
     <t>married</t>
   </si>
   <si>
@@ -273,6 +270,21 @@
   </si>
   <si>
     <t>Angular</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>Bali</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>Jogjakarta</t>
+  </si>
+  <si>
+    <t>Bandung</t>
   </si>
 </sst>
 </file>
@@ -612,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O14"/>
+  <dimension ref="A2:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +646,7 @@
     <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -680,8 +692,11 @@
       <c r="O2" t="s">
         <v>13</v>
       </c>
+      <c r="P2" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -710,7 +725,7 @@
         <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
         <v>21</v>
@@ -727,8 +742,11 @@
       <c r="O3" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="P3" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -736,7 +754,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -745,19 +763,19 @@
         <v>29371</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
         <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
       </c>
       <c r="H4" s="2">
         <v>68129031389</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K4" t="s">
         <v>21</v>
@@ -766,33 +784,36 @@
         <v>42195</v>
       </c>
       <c r="M4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
         <v>31</v>
       </c>
-      <c r="N4" t="s">
-        <v>32</v>
-      </c>
       <c r="O4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="P4" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
         <v>49</v>
       </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="1">
         <v>33219</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
@@ -804,74 +825,86 @@
         <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
       </c>
       <c r="L5" s="1">
         <v>41312</v>
       </c>
       <c r="M5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="P5" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
         <v>51</v>
       </c>
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="1">
         <v>30708</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="2">
         <v>62832837912</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
       </c>
       <c r="L6" s="1">
         <v>40918</v>
       </c>
       <c r="M6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="P6" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
         <v>47</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -880,51 +913,57 @@
         <v>29138</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="2">
         <v>623273289</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J7" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
       </c>
       <c r="L7" s="1">
         <v>41931</v>
       </c>
       <c r="M7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="P7" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
         <v>53</v>
       </c>
-      <c r="C8" t="s">
-        <v>54</v>
-      </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="1">
         <v>30651</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G8" t="s">
         <v>17</v>
@@ -933,33 +972,39 @@
         <v>628780082</v>
       </c>
       <c r="I8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J8" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="K8" t="s">
+        <v>21</v>
       </c>
       <c r="L8" s="1">
         <v>42571</v>
       </c>
       <c r="M8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" t="s">
         <v>41</v>
       </c>
-      <c r="N8" t="s">
-        <v>42</v>
-      </c>
       <c r="O8" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="P8" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
         <v>55</v>
-      </c>
-      <c r="C9" t="s">
-        <v>56</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -968,7 +1013,7 @@
         <v>33344</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9" t="s">
         <v>17</v>
@@ -977,33 +1022,39 @@
         <v>628273182230</v>
       </c>
       <c r="I9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J9" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
       </c>
       <c r="L9" s="1">
         <v>42031</v>
       </c>
       <c r="M9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="P9" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
         <v>59</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
@@ -1012,19 +1063,22 @@
         <v>34552</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" s="2">
         <v>6512362131</v>
       </c>
       <c r="I10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J10" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
       </c>
       <c r="L10" s="1">
         <v>40981</v>
@@ -1033,21 +1087,24 @@
         <v>22</v>
       </c>
       <c r="N10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="P10" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
         <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>62</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
@@ -1056,7 +1113,7 @@
         <v>34021</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G11" t="s">
         <v>17</v>
@@ -1068,39 +1125,45 @@
         <v>20</v>
       </c>
       <c r="J11" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
       </c>
       <c r="L11" s="1">
         <v>42750</v>
       </c>
       <c r="M11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N11" t="s">
         <v>23</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="P11" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
         <v>57</v>
       </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="1">
         <v>34691</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G12" t="s">
         <v>17</v>
@@ -1112,30 +1175,36 @@
         <v>20</v>
       </c>
       <c r="J12" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="K12" t="s">
+        <v>21</v>
       </c>
       <c r="L12" s="1">
         <v>42793</v>
       </c>
       <c r="M12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="P12" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
         <v>63</v>
-      </c>
-      <c r="C13" t="s">
-        <v>64</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
@@ -1144,42 +1213,48 @@
         <v>31195</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" s="2">
         <v>628271230090</v>
       </c>
       <c r="I13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J13" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="K13" t="s">
+        <v>21</v>
       </c>
       <c r="L13" s="1">
         <v>42454</v>
       </c>
       <c r="M13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="P13" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
         <v>64</v>
-      </c>
-      <c r="C14" t="s">
-        <v>65</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1188,10 +1263,10 @@
         <v>33922</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14" s="2">
         <v>6231288213</v>
@@ -1200,7 +1275,10 @@
         <v>20</v>
       </c>
       <c r="J14" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="K14" t="s">
+        <v>21</v>
       </c>
       <c r="L14" s="1">
         <v>40554</v>
@@ -1209,10 +1287,13 @@
         <v>22</v>
       </c>
       <c r="N14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="P14" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>